<commit_message>
Updates to excel files
</commit_message>
<xml_diff>
--- a/IA_CCBS_BANK_SIDE/AccountOther/LoanAccountOpening_InstantProcess.xlsx
+++ b/IA_CCBS_BANK_SIDE/AccountOther/LoanAccountOpening_InstantProcess.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sw\Relational_Files\Interfaces\Interfaces_new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sw\Relational_Files\Interfaces_aa\Interfaces\IA_CCBS_BANK_SIDE\AccountOther\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412A292E-FF4E-4116-AE5F-3D9F0D537B19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB67502-D788-422B-A7B5-FE1FFC3D3460}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{68F28061-2ECD-4B0A-AB1D-3A449686159F}"/>
   </bookViews>
@@ -99,9 +99,6 @@
     <t>Last Update</t>
   </si>
   <si>
-    <t>Sept 9 2023</t>
-  </si>
-  <si>
     <t>decimal (15,2)</t>
   </si>
   <si>
@@ -337,6 +334,9 @@
   </si>
   <si>
     <t>profitsaccountcd</t>
+  </si>
+  <si>
+    <t>Sept 6 2023</t>
   </si>
 </sst>
 </file>
@@ -667,13 +667,285 @@
   <dxfs count="24">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -722,288 +994,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="161"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1273,6 +1263,16 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1287,32 +1287,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A6ACF92C-1104-4C93-8F8B-A938A4312D3B}" name="Table2" displayName="Table2" ref="A1:F30" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A6ACF92C-1104-4C93-8F8B-A938A4312D3B}" name="Table2" displayName="Table2" ref="A1:F30" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <sortState ref="A2:F30">
     <sortCondition ref="A2"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{85C05364-CF34-480B-84A9-1E752A61B8E7}" name="Seq" dataDxfId="19" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{B74F6632-9589-464E-84C1-0830E8F1F8D8}" name="Description" dataDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{9572A906-3602-4DBD-9459-262F500E1D9A}" name="iApply" dataDxfId="17" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{88CBB51C-2237-4EBC-90F4-9EFEDD4BEC32}" name="Data Type" dataDxfId="16" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{543BB0EE-DFCA-4B94-847F-73C897029E52}" name="Entities" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{2E373EFE-D19B-41E5-92FD-B165DCC3E8F5}" name="Notes" dataDxfId="14" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{85C05364-CF34-480B-84A9-1E752A61B8E7}" name="Seq" dataDxfId="18" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{B74F6632-9589-464E-84C1-0830E8F1F8D8}" name="Description" dataDxfId="17" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{9572A906-3602-4DBD-9459-262F500E1D9A}" name="iApply" dataDxfId="16" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{88CBB51C-2237-4EBC-90F4-9EFEDD4BEC32}" name="Data Type" dataDxfId="15" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{543BB0EE-DFCA-4B94-847F-73C897029E52}" name="Entities" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{2E373EFE-D19B-41E5-92FD-B165DCC3E8F5}" name="Notes" dataDxfId="13" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F11F741B-5D22-4BBF-9B93-935C1585CBED}" name="Table22" displayName="Table22" ref="A1:F9" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F11F741B-5D22-4BBF-9B93-935C1585CBED}" name="Table22" displayName="Table22" ref="A1:F9" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="A1:F9" xr:uid="{FE54AB27-2F61-427B-9D73-DA77A59601D2}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F8F1211F-EA34-4B44-896A-D528AAFAE184}" name="Seq" dataDxfId="9" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{03B9C3AE-C4F7-4512-A115-C772590AED2F}" name="Description" dataDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{86EE5336-821C-4C56-8460-1456EB6E1740}" name="iApply" dataDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{33764DB6-8011-4E1D-A09A-295251C6CCE7}" name="Data Type" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{AC1C2596-97D1-445C-B651-3EAD2A6C7064}" name="Entities" dataDxfId="6" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{8FD2DAF4-1939-4C6D-BEB9-074AFC032812}" name="Notes" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{F8F1211F-EA34-4B44-896A-D528AAFAE184}" name="Seq" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{03B9C3AE-C4F7-4512-A115-C772590AED2F}" name="Description" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{86EE5336-821C-4C56-8460-1456EB6E1740}" name="iApply" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{33764DB6-8011-4E1D-A09A-295251C6CCE7}" name="Data Type" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{AC1C2596-97D1-445C-B651-3EAD2A6C7064}" name="Entities" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{8FD2DAF4-1939-4C6D-BEB9-074AFC032812}" name="Notes" dataDxfId="0" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1618,7 +1618,7 @@
   <dimension ref="B2:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,7 +1647,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -1663,7 +1663,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -1691,7 +1691,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
@@ -1707,7 +1707,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
@@ -1766,13 +1766,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" s="27"/>
     </row>
@@ -1781,16 +1781,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="D3" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="26" t="s">
-        <v>36</v>
-      </c>
       <c r="E3" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" s="27"/>
     </row>
@@ -1799,16 +1799,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>37</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>38</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" s="27"/>
     </row>
@@ -1817,16 +1817,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>39</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>40</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" s="27"/>
     </row>
@@ -1835,16 +1835,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="26" t="s">
         <v>41</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>42</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6" s="27"/>
     </row>
@@ -1853,16 +1853,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="26" t="s">
         <v>43</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>44</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" s="28"/>
     </row>
@@ -1871,16 +1871,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="26" t="s">
-        <v>46</v>
-      </c>
       <c r="D8" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="27"/>
     </row>
@@ -1889,16 +1889,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="28"/>
     </row>
@@ -1907,16 +1907,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F10" s="27"/>
     </row>
@@ -1925,16 +1925,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="27"/>
     </row>
@@ -1943,16 +1943,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="26" t="s">
-        <v>50</v>
-      </c>
       <c r="D12" s="26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="27"/>
     </row>
@@ -1961,16 +1961,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="26" t="s">
         <v>51</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>52</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="27"/>
     </row>
@@ -1979,16 +1979,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="26" t="s">
-        <v>54</v>
-      </c>
       <c r="D14" s="26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="27"/>
     </row>
@@ -1997,16 +1997,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="26" t="s">
         <v>55</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>56</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" s="27"/>
     </row>
@@ -2015,16 +2015,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="26" t="s">
         <v>57</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>58</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16" s="27"/>
     </row>
@@ -2033,16 +2033,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="26" t="s">
         <v>59</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>60</v>
       </c>
       <c r="D17" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" s="27"/>
     </row>
@@ -2051,16 +2051,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="26" t="s">
         <v>61</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>62</v>
       </c>
       <c r="D18" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" s="27"/>
     </row>
@@ -2069,16 +2069,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="26" t="s">
         <v>63</v>
-      </c>
-      <c r="C19" s="26" t="s">
-        <v>64</v>
       </c>
       <c r="D19" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F19" s="27"/>
     </row>
@@ -2087,16 +2087,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="26" t="s">
         <v>65</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>66</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F20" s="27"/>
     </row>
@@ -2105,16 +2105,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="26" t="s">
         <v>67</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>68</v>
       </c>
       <c r="D21" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F21" s="27"/>
     </row>
@@ -2123,16 +2123,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="26" t="s">
         <v>69</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>70</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F22" s="27"/>
     </row>
@@ -2141,16 +2141,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="26" t="s">
         <v>71</v>
-      </c>
-      <c r="C23" s="26" t="s">
-        <v>72</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F23" s="27"/>
     </row>
@@ -2159,16 +2159,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D24" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F24" s="27"/>
     </row>
@@ -2177,16 +2177,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="26" t="s">
         <v>74</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>75</v>
       </c>
       <c r="D25" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F25" s="27"/>
     </row>
@@ -2196,13 +2196,13 @@
       </c>
       <c r="B26" s="26"/>
       <c r="C26" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D26" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F26" s="27">
         <v>0</v>
@@ -2213,16 +2213,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D27" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F27" s="28"/>
     </row>
@@ -2231,16 +2231,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="26" t="s">
         <v>78</v>
-      </c>
-      <c r="C28" s="26" t="s">
-        <v>79</v>
       </c>
       <c r="D28" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F28" s="27"/>
     </row>
@@ -2249,16 +2249,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="26" t="s">
         <v>80</v>
-      </c>
-      <c r="C29" s="26" t="s">
-        <v>81</v>
       </c>
       <c r="D29" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F29" s="27"/>
     </row>
@@ -2267,16 +2267,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F30" s="27"/>
     </row>
@@ -2792,7 +2792,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2845,16 +2845,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>27</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>28</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F2" s="27"/>
     </row>
@@ -2863,16 +2863,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="D3" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="26" t="s">
         <v>85</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>86</v>
       </c>
       <c r="F3" s="27"/>
     </row>
@@ -2881,16 +2881,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>87</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>88</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F4" s="27"/>
     </row>
@@ -2899,16 +2899,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="D5" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>91</v>
-      </c>
       <c r="E5" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F5" s="27"/>
     </row>
@@ -2917,16 +2917,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="D6" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D6" s="30" t="s">
-        <v>94</v>
-      </c>
       <c r="E6" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F6" s="30">
         <v>1</v>
@@ -2937,16 +2937,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>96</v>
-      </c>
       <c r="D7" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F7" s="30">
         <v>2</v>
@@ -2957,16 +2957,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="D8" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="26" t="s">
         <v>98</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>99</v>
       </c>
       <c r="F8" s="27"/>
     </row>
@@ -2975,16 +2975,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="30" t="s">
         <v>100</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>101</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F9" s="27"/>
     </row>
@@ -3488,11 +3488,11 @@
     <row r="95" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="C2:C9">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:D1048576 C1">
-    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>